<commit_message>
Refactor users and courses import
</commit_message>
<xml_diff>
--- a/spec/data/courses.xlsx
+++ b/spec/data/courses.xlsx
@@ -25,7 +25,7 @@
     <t>大钢1</t>
   </si>
   <si>
-    <t>desc</t>
+    <t>课程编号</t>
   </si>
   <si>
     <t>简介2</t>
@@ -34,15 +34,18 @@
     <t>大钢2</t>
   </si>
   <si>
+    <t>课程名称</t>
+  </si>
+  <si>
+    <t>描述</t>
+  </si>
+  <si>
     <t>简介3</t>
   </si>
   <si>
     <t>大钢3</t>
   </si>
   <si>
-    <t>cid</t>
-  </si>
-  <si>
     <t>数学1</t>
   </si>
   <si>
@@ -52,10 +55,7 @@
     <t>数学2</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>syllabus</t>
+    <t>教学大钢</t>
   </si>
 </sst>
 </file>
@@ -492,13 +492,13 @@
   <sheetData>
     <row r="1" ht="12.1">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="2" ht="12.1">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="n">
         <v>111</v>
@@ -520,7 +520,7 @@
     </row>
     <row r="3" ht="12.1">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="n">
         <v>112</v>
@@ -534,16 +534,16 @@
     </row>
     <row r="4" ht="12.1">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
         <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>